<commit_message>
renamings, german removed, similarity search gui updated, lot number to be essential for import
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace.xlsx
@@ -10,9 +10,8 @@
     <sheet name="Stations" sheetId="2" r:id="rId1"/>
     <sheet name="BackTracing" sheetId="5" r:id="rId2"/>
     <sheet name="Opt_ForwardTracing" sheetId="1" r:id="rId3"/>
-    <sheet name="Opt_Sampling" sheetId="4" r:id="rId4"/>
-    <sheet name="LookUp" sheetId="3" r:id="rId5"/>
-    <sheet name="Help" sheetId="6" r:id="rId6"/>
+    <sheet name="LookUp" sheetId="3" r:id="rId4"/>
+    <sheet name="Help" sheetId="6" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Stations!$A$1:$J$8</definedName>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="118">
   <si>
     <t>Supplier</t>
   </si>
@@ -249,9 +248,6 @@
   </si>
   <si>
     <t>Sampling</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> , </t>
   </si>
   <si>
     <t>Reporting Remark</t>
@@ -2451,7 +2447,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="54" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F1" s="54" t="s">
         <v>7</v>
@@ -2469,7 +2465,7 @@
         <v>12</v>
       </c>
       <c r="K1" s="58" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="L1" s="59"/>
       <c r="M1" s="59"/>
@@ -2517,9 +2513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2543,7 +2537,7 @@
   <sheetData>
     <row r="1" spans="1:21" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="30" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B1" s="94"/>
       <c r="C1" s="32" t="e">
@@ -2568,7 +2562,7 @@
     </row>
     <row r="3" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="95" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B3" s="96"/>
       <c r="C3" s="96"/>
@@ -2582,7 +2576,7 @@
       <c r="K3" s="96"/>
       <c r="L3" s="96"/>
       <c r="M3" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N3" s="68"/>
       <c r="O3" s="68"/>
@@ -2601,27 +2595,27 @@
         <v>2</v>
       </c>
       <c r="C4" s="108" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D4" s="109"/>
       <c r="E4" s="110"/>
       <c r="F4" s="108" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="109"/>
       <c r="H4" s="110"/>
       <c r="I4" s="106" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J4" s="107"/>
       <c r="K4" s="113" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="L4" s="115" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="M4" s="118" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="N4" s="51"/>
       <c r="O4" s="51"/>
@@ -2636,28 +2630,28 @@
       <c r="A5" s="98"/>
       <c r="B5" s="114"/>
       <c r="C5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="D5" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="E5" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="F5" s="26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G5" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="H5" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>102</v>
+      </c>
+      <c r="J5" s="21" t="s">
         <v>79</v>
-      </c>
-      <c r="F5" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="G5" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="H5" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="I5" s="21" t="s">
-        <v>103</v>
-      </c>
-      <c r="J5" s="21" t="s">
-        <v>80</v>
       </c>
       <c r="K5" s="114"/>
       <c r="L5" s="116"/>
@@ -2709,7 +2703,7 @@
     </row>
     <row r="8" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="103" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B8" s="104"/>
       <c r="C8" s="105"/>
@@ -2731,7 +2725,7 @@
         <v>13</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D9" s="22"/>
     </row>
@@ -2749,7 +2743,7 @@
     </row>
     <row r="12" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="103" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B12" s="111"/>
       <c r="C12" s="112"/>
@@ -2763,7 +2757,7 @@
       <c r="K12" s="62"/>
       <c r="L12" s="62"/>
       <c r="M12" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N12" s="68"/>
       <c r="O12" s="68"/>
@@ -2776,20 +2770,20 @@
     </row>
     <row r="13" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="122" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B13" s="120" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C13" s="121"/>
       <c r="M13" s="97" t="s">
+        <v>107</v>
+      </c>
+      <c r="N13" s="99" t="s">
         <v>108</v>
       </c>
-      <c r="N13" s="99" t="s">
-        <v>109</v>
-      </c>
       <c r="O13" s="99" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="P13" s="101" t="s">
         <v>72</v>
@@ -2803,10 +2797,10 @@
     <row r="14" spans="1:21" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="123"/>
       <c r="B14" s="47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C14" s="63" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M14" s="98"/>
       <c r="N14" s="100"/>
@@ -2848,7 +2842,7 @@
     </row>
     <row r="17" spans="1:21" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="95" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B17" s="96"/>
       <c r="C17" s="96"/>
@@ -2862,7 +2856,7 @@
       <c r="K17" s="96"/>
       <c r="L17" s="96"/>
       <c r="M17" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N17" s="68"/>
       <c r="O17" s="68"/>
@@ -2875,33 +2869,33 @@
     </row>
     <row r="18" spans="1:21" s="14" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="124" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B18" s="126" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C18" s="128" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="D18" s="109"/>
       <c r="E18" s="110"/>
       <c r="F18" s="129" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G18" s="130"/>
       <c r="H18" s="131"/>
       <c r="I18" s="128" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="J18" s="110"/>
       <c r="K18" s="126" t="s">
         <v>0</v>
       </c>
       <c r="L18" s="132" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M18" s="125" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="N18" s="52"/>
       <c r="O18" s="52"/>
@@ -2916,28 +2910,28 @@
       <c r="A19" s="98"/>
       <c r="B19" s="127"/>
       <c r="C19" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="F19" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>77</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>78</v>
+      </c>
+      <c r="I19" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="J19" s="16" t="s">
         <v>79</v>
-      </c>
-      <c r="F19" s="27" t="s">
-        <v>77</v>
-      </c>
-      <c r="G19" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="H19" s="27" t="s">
-        <v>79</v>
-      </c>
-      <c r="I19" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="J19" s="16" t="s">
-        <v>80</v>
       </c>
       <c r="K19" s="114"/>
       <c r="L19" s="116"/>
@@ -5036,34 +5030,34 @@
         <v>2</v>
       </c>
       <c r="B1" s="137" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="138"/>
       <c r="D1" s="138"/>
       <c r="E1" s="137" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F1" s="138"/>
       <c r="G1" s="133" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="2" spans="1:7" s="40" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="136"/>
       <c r="B2" s="90" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="90" t="s">
         <v>77</v>
       </c>
-      <c r="C2" s="90" t="s">
+      <c r="D2" s="90" t="s">
         <v>78</v>
       </c>
-      <c r="D2" s="90" t="s">
+      <c r="E2" s="90" t="s">
+        <v>102</v>
+      </c>
+      <c r="F2" s="90" t="s">
         <v>79</v>
-      </c>
-      <c r="E2" s="90" t="s">
-        <v>103</v>
-      </c>
-      <c r="F2" s="90" t="s">
-        <v>80</v>
       </c>
       <c r="G2" s="134"/>
     </row>
@@ -5107,38 +5101,6 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="L1:L2"/>
-  <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="4" width="11.42578125" style="2"/>
-    <col min="5" max="5" width="10.42578125" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" style="2"/>
-    <col min="7" max="7" width="10.28515625" style="2" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" style="2" customWidth="1"/>
-    <col min="9" max="11" width="11.42578125" style="2"/>
-    <col min="12" max="12" width="10.42578125" style="2" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="2"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="12:12" s="14" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="12:12" x14ac:dyDescent="0.25">
-      <c r="L2" s="2" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5173,13 +5135,13 @@
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>69</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -5187,13 +5149,13 @@
         <v>16</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>68</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -5201,13 +5163,13 @@
         <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -5215,7 +5177,7 @@
         <v>18</v>
       </c>
       <c r="B5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>67</v>
@@ -5229,7 +5191,7 @@
         <v>19</v>
       </c>
       <c r="B6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>62</v>
@@ -5243,7 +5205,7 @@
         <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>14</v>
@@ -5257,7 +5219,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>63</v>
@@ -5271,7 +5233,7 @@
         <v>22</v>
       </c>
       <c r="B9" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>64</v>
@@ -5285,7 +5247,7 @@
         <v>23</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>65</v>
@@ -5299,7 +5261,7 @@
         <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>66</v>
@@ -5438,7 +5400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B6"/>
   <sheetViews>
@@ -5460,7 +5422,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5473,12 +5435,12 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
"Replace files?"-dialog added for template generator
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace.xlsx
@@ -1843,54 +1843,147 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="30" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="30" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1918,140 +2011,47 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="30" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="30" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2555,7 +2555,6 @@
       <c r="A3" s="89"/>
     </row>
   </sheetData>
-  <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
   <autoFilter ref="A1:J8"/>
   <dataValidations count="3">
     <dataValidation sqref="E2:E3"/>
@@ -2588,7 +2587,7 @@
     <col min="8" max="8" width="7.85546875" style="21" customWidth="1"/>
     <col min="9" max="9" width="10.5703125" style="21" customWidth="1"/>
     <col min="10" max="10" width="13.28515625" style="21" customWidth="1"/>
-    <col min="11" max="11" width="16" style="21" customWidth="1"/>
+    <col min="11" max="11" width="36" style="21" customWidth="1"/>
     <col min="12" max="12" width="16.140625" style="21" customWidth="1"/>
     <col min="13" max="13" width="16.140625" style="24" customWidth="1"/>
     <col min="14" max="14" width="17.42578125" style="21" customWidth="1"/>
@@ -2598,11 +2597,11 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="21" customHeight="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="118"/>
+      <c r="B1" s="110"/>
+      <c r="C1" s="111"/>
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="37"/>
@@ -2665,20 +2664,20 @@
       <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:22" s="42" customFormat="1" ht="21" customHeight="1" thickBot="1">
-      <c r="A7" s="143" t="s">
+      <c r="A7" s="137" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="144"/>
-      <c r="C7" s="144"/>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="144"/>
+      <c r="B7" s="138"/>
+      <c r="C7" s="138"/>
+      <c r="D7" s="138"/>
+      <c r="E7" s="138"/>
+      <c r="F7" s="138"/>
+      <c r="G7" s="138"/>
+      <c r="H7" s="138"/>
+      <c r="I7" s="138"/>
+      <c r="J7" s="138"/>
+      <c r="K7" s="138"/>
+      <c r="L7" s="138"/>
       <c r="M7" s="71"/>
       <c r="N7" s="70" t="s">
         <v>32</v>
@@ -2693,48 +2692,48 @@
       <c r="V7" s="73"/>
     </row>
     <row r="8" spans="1:22" ht="18.75" customHeight="1">
-      <c r="A8" s="133" t="s">
+      <c r="A8" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="116" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="125"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="121" t="s">
+      <c r="D8" s="117"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="113" t="s">
         <v>39</v>
       </c>
-      <c r="G8" s="122"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="119" t="s">
+      <c r="G8" s="114"/>
+      <c r="H8" s="115"/>
+      <c r="I8" s="112" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="120"/>
-      <c r="K8" s="129" t="s">
+      <c r="J8" s="98"/>
+      <c r="K8" s="121" t="s">
         <v>41</v>
       </c>
-      <c r="L8" s="112" t="s">
+      <c r="L8" s="146" t="s">
         <v>41</v>
       </c>
-      <c r="M8" s="131" t="s">
+      <c r="M8" s="123" t="s">
         <v>45</v>
       </c>
-      <c r="N8" s="135"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="103"/>
+      <c r="N8" s="127"/>
+      <c r="O8" s="135"/>
+      <c r="P8" s="135"/>
+      <c r="Q8" s="135"/>
+      <c r="R8" s="135"/>
+      <c r="S8" s="135"/>
+      <c r="T8" s="135"/>
+      <c r="U8" s="135"/>
+      <c r="V8" s="148"/>
     </row>
     <row r="9" spans="1:22" ht="17.25" customHeight="1">
-      <c r="A9" s="134"/>
-      <c r="B9" s="138"/>
+      <c r="A9" s="126"/>
+      <c r="B9" s="130"/>
       <c r="C9" s="74" t="s">
         <v>20</v>
       </c>
@@ -2759,18 +2758,18 @@
       <c r="J9" s="76" t="s">
         <v>23</v>
       </c>
-      <c r="K9" s="130"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="132"/>
-      <c r="N9" s="136"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="100"/>
-      <c r="Q9" s="100"/>
-      <c r="R9" s="100"/>
-      <c r="S9" s="100"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="100"/>
-      <c r="V9" s="104"/>
+      <c r="K9" s="122"/>
+      <c r="L9" s="147"/>
+      <c r="M9" s="124"/>
+      <c r="N9" s="128"/>
+      <c r="O9" s="136"/>
+      <c r="P9" s="136"/>
+      <c r="Q9" s="136"/>
+      <c r="R9" s="136"/>
+      <c r="S9" s="136"/>
+      <c r="T9" s="136"/>
+      <c r="U9" s="136"/>
+      <c r="V9" s="149"/>
     </row>
     <row r="10" spans="1:22" s="42" customFormat="1" ht="21" customHeight="1">
       <c r="A10" s="49"/>
@@ -2811,11 +2810,11 @@
       <c r="M11" s="42"/>
     </row>
     <row r="12" spans="1:22" ht="21" customHeight="1" thickBot="1">
-      <c r="A12" s="116" t="s">
+      <c r="A12" s="109" t="s">
         <v>29</v>
       </c>
-      <c r="B12" s="127"/>
-      <c r="C12" s="128"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="120"/>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
@@ -2839,34 +2838,34 @@
       <c r="V12" s="39"/>
     </row>
     <row r="13" spans="1:22" ht="18" customHeight="1">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="133" t="s">
         <v>35</v>
       </c>
-      <c r="B13" s="139" t="s">
+      <c r="B13" s="131" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="140"/>
+      <c r="C13" s="132"/>
       <c r="M13" s="60"/>
-      <c r="N13" s="108" t="s">
+      <c r="N13" s="142" t="s">
         <v>36</v>
       </c>
-      <c r="O13" s="110" t="s">
+      <c r="O13" s="144" t="s">
         <v>37</v>
       </c>
-      <c r="P13" s="110" t="s">
+      <c r="P13" s="144" t="s">
         <v>25</v>
       </c>
-      <c r="Q13" s="114" t="s">
+      <c r="Q13" s="107" t="s">
         <v>18</v>
       </c>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="98"/>
-      <c r="U13" s="99"/>
-      <c r="V13" s="101"/>
+      <c r="R13" s="150"/>
+      <c r="S13" s="150"/>
+      <c r="T13" s="152"/>
+      <c r="U13" s="135"/>
+      <c r="V13" s="153"/>
     </row>
     <row r="14" spans="1:22" ht="17.25" customHeight="1">
-      <c r="A14" s="142"/>
+      <c r="A14" s="134"/>
       <c r="B14" s="77" t="s">
         <v>33</v>
       </c>
@@ -2874,15 +2873,15 @@
         <v>23</v>
       </c>
       <c r="M14" s="60"/>
-      <c r="N14" s="109"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="111"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="97"/>
-      <c r="S14" s="97"/>
-      <c r="T14" s="97"/>
-      <c r="U14" s="100"/>
-      <c r="V14" s="102"/>
+      <c r="N14" s="143"/>
+      <c r="O14" s="145"/>
+      <c r="P14" s="145"/>
+      <c r="Q14" s="108"/>
+      <c r="R14" s="151"/>
+      <c r="S14" s="151"/>
+      <c r="T14" s="151"/>
+      <c r="U14" s="136"/>
+      <c r="V14" s="154"/>
     </row>
     <row r="15" spans="1:22" ht="21" customHeight="1">
       <c r="A15" s="18"/>
@@ -2914,20 +2913,20 @@
       <c r="M16" s="48"/>
     </row>
     <row r="17" spans="1:22" ht="21" customHeight="1">
-      <c r="A17" s="105" t="s">
+      <c r="A17" s="139" t="s">
         <v>31</v>
       </c>
-      <c r="B17" s="106"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="107"/>
+      <c r="B17" s="140"/>
+      <c r="C17" s="140"/>
+      <c r="D17" s="140"/>
+      <c r="E17" s="140"/>
+      <c r="F17" s="140"/>
+      <c r="G17" s="140"/>
+      <c r="H17" s="140"/>
+      <c r="I17" s="140"/>
+      <c r="J17" s="140"/>
+      <c r="K17" s="140"/>
+      <c r="L17" s="141"/>
       <c r="M17" s="79"/>
       <c r="N17" s="51" t="s">
         <v>32</v>
@@ -2942,48 +2941,48 @@
       <c r="V17" s="45"/>
     </row>
     <row r="18" spans="1:22" s="46" customFormat="1" ht="25.5" customHeight="1">
-      <c r="A18" s="145" t="s">
+      <c r="A18" s="92" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="149" t="s">
+      <c r="B18" s="96" t="s">
         <v>27</v>
       </c>
-      <c r="C18" s="151" t="s">
+      <c r="C18" s="99" t="s">
         <v>38</v>
       </c>
-      <c r="D18" s="154"/>
-      <c r="E18" s="152"/>
-      <c r="F18" s="153" t="s">
+      <c r="D18" s="102"/>
+      <c r="E18" s="100"/>
+      <c r="F18" s="101" t="s">
         <v>40</v>
       </c>
-      <c r="G18" s="154"/>
-      <c r="H18" s="152"/>
-      <c r="I18" s="151" t="s">
+      <c r="G18" s="102"/>
+      <c r="H18" s="100"/>
+      <c r="I18" s="99" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="152"/>
-      <c r="K18" s="149" t="s">
+      <c r="J18" s="100"/>
+      <c r="K18" s="96" t="s">
         <v>0</v>
       </c>
-      <c r="L18" s="157" t="s">
+      <c r="L18" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="M18" s="155" t="s">
+      <c r="M18" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="N18" s="147"/>
-      <c r="O18" s="92"/>
-      <c r="P18" s="92"/>
-      <c r="Q18" s="92"/>
-      <c r="R18" s="92"/>
-      <c r="S18" s="92"/>
-      <c r="T18" s="92"/>
-      <c r="U18" s="92"/>
-      <c r="V18" s="94"/>
+      <c r="N18" s="94"/>
+      <c r="O18" s="155"/>
+      <c r="P18" s="155"/>
+      <c r="Q18" s="155"/>
+      <c r="R18" s="155"/>
+      <c r="S18" s="155"/>
+      <c r="T18" s="155"/>
+      <c r="U18" s="155"/>
+      <c r="V18" s="157"/>
     </row>
     <row r="19" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1">
-      <c r="A19" s="146"/>
-      <c r="B19" s="150"/>
+      <c r="A19" s="93"/>
+      <c r="B19" s="97"/>
       <c r="C19" s="80" t="s">
         <v>20</v>
       </c>
@@ -3008,18 +3007,18 @@
       <c r="J19" s="80" t="s">
         <v>23</v>
       </c>
-      <c r="K19" s="120"/>
-      <c r="L19" s="158"/>
-      <c r="M19" s="156"/>
-      <c r="N19" s="148"/>
-      <c r="O19" s="93"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="93"/>
-      <c r="R19" s="93"/>
-      <c r="S19" s="93"/>
-      <c r="T19" s="93"/>
-      <c r="U19" s="93"/>
-      <c r="V19" s="95"/>
+      <c r="K19" s="98"/>
+      <c r="L19" s="106"/>
+      <c r="M19" s="104"/>
+      <c r="N19" s="95"/>
+      <c r="O19" s="156"/>
+      <c r="P19" s="156"/>
+      <c r="Q19" s="156"/>
+      <c r="R19" s="156"/>
+      <c r="S19" s="156"/>
+      <c r="T19" s="156"/>
+      <c r="U19" s="156"/>
+      <c r="V19" s="158"/>
     </row>
     <row r="20" spans="1:22" ht="21" customHeight="1">
       <c r="A20" s="64"/>
@@ -5090,17 +5089,32 @@
       <c r="M106" s="21"/>
     </row>
   </sheetData>
-  <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="49">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="T18:T19"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="V18:V19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
     <mergeCell ref="Q13:Q14"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="I8:J8"/>
@@ -5116,31 +5130,15 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="T18:T19"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="V18:V19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="L18:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5184,7 +5182,7 @@
       <c r="G1" s="159" t="s">
         <v>41</v>
       </c>
-      <c r="H1" s="112" t="s">
+      <c r="H1" s="146" t="s">
         <v>41</v>
       </c>
     </row>
@@ -11197,7 +11195,6 @@
       </c>
     </row>
   </sheetData>
-  <sheetProtection password="CF7A" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="5">
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="A1:A2"/>

</xml_diff>

<commit_message>
Templates adapted to Reporting Date separation
</commit_message>
<xml_diff>
--- a/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace.xlsx
+++ b/de.bund.bfr.knime.openkrise.db/src/de/bund/bfr/knime/openkrise/db/imports/custom/bfrnewformat/BfR_Format_Backtrace.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="52">
   <si>
     <t>Supplier</t>
   </si>
@@ -63,9 +63,6 @@
   </si>
   <si>
     <t>Type of business</t>
-  </si>
-  <si>
-    <t>Reporting Date</t>
   </si>
   <si>
     <t>Type of Business</t>
@@ -183,6 +180,9 @@
   </si>
   <si>
     <t>Optionaly it is possible to give information on further yet unknown forwards deliveries for each requested lot</t>
+  </si>
+  <si>
+    <t>Reporting Date: Day</t>
   </si>
 </sst>
 </file>
@@ -659,7 +659,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="62">
+  <borders count="63">
     <border>
       <left/>
       <right/>
@@ -1464,6 +1464,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1581,7 +1592,7 @@
     <xf numFmtId="0" fontId="37" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="38" fillId="31" borderId="61" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="167">
+  <cellXfs count="168">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyProtection="1">
       <protection locked="0"/>
@@ -1855,54 +1866,148 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="30" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="30" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="30" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="10" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1930,140 +2035,47 @@
     <xf numFmtId="0" fontId="34" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="54" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="54" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="30" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="2" fillId="30" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="36" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="30" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="59" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="51" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
     <xf numFmtId="49" fontId="6" fillId="4" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2082,9 +2094,11 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="114">
     <cellStyle name="20% - Accent1 2" xfId="4"/>
@@ -2533,7 +2547,7 @@
         <v>10</v>
       </c>
       <c r="E1" s="84" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F1" s="84" t="s">
         <v>7</v>
@@ -2551,7 +2565,7 @@
         <v>12</v>
       </c>
       <c r="K1" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="16"/>
       <c r="M1" s="16"/>
@@ -2587,16 +2601,16 @@
   <dimension ref="A1:V106"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C1"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.7109375" style="21" customWidth="1"/>
     <col min="2" max="2" width="24" style="21" customWidth="1"/>
-    <col min="3" max="3" width="11.28515625" style="21" customWidth="1"/>
-    <col min="4" max="4" width="7" style="21" customWidth="1"/>
-    <col min="5" max="5" width="6.5703125" style="21" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" style="21" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" style="21" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" style="21" customWidth="1"/>
     <col min="6" max="6" width="6" style="21" customWidth="1"/>
     <col min="7" max="7" width="7.5703125" style="21" customWidth="1"/>
     <col min="8" max="8" width="7.85546875" style="21" customWidth="1"/>
@@ -2611,14 +2625,14 @@
     <col min="17" max="16384" width="11.42578125" style="21"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="116" t="s">
-        <v>26</v>
-      </c>
-      <c r="B1" s="117"/>
-      <c r="C1" s="118"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
+    <row r="1" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="165" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="166"/>
+      <c r="C1" s="166"/>
+      <c r="D1" s="167"/>
+      <c r="E1" s="167"/>
       <c r="F1" s="37"/>
       <c r="G1" s="37"/>
       <c r="H1" s="37"/>
@@ -2633,19 +2647,25 @@
         <v>11</v>
       </c>
       <c r="B2" s="67" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="41"/>
+        <v>51</v>
+      </c>
+      <c r="C2" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="E2" s="68" t="s">
+        <v>17</v>
+      </c>
       <c r="M2" s="60"/>
     </row>
     <row r="3" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31"/>
       <c r="B3" s="32"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="41"/>
+      <c r="C3" s="52"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="43"/>
       <c r="M3" s="60"/>
     </row>
     <row r="4" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
@@ -2657,7 +2677,7 @@
     </row>
     <row r="5" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="69" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="59"/>
       <c r="C5" s="58" t="e">
@@ -2679,23 +2699,23 @@
       <c r="M6" s="21"/>
     </row>
     <row r="7" spans="1:22" s="42" customFormat="1" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="143" t="s">
-        <v>28</v>
-      </c>
-      <c r="B7" s="144"/>
-      <c r="C7" s="144"/>
-      <c r="D7" s="144"/>
-      <c r="E7" s="144"/>
-      <c r="F7" s="144"/>
-      <c r="G7" s="144"/>
-      <c r="H7" s="144"/>
-      <c r="I7" s="144"/>
-      <c r="J7" s="144"/>
-      <c r="K7" s="144"/>
-      <c r="L7" s="144"/>
+      <c r="A7" s="136" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="137"/>
+      <c r="C7" s="137"/>
+      <c r="D7" s="137"/>
+      <c r="E7" s="137"/>
+      <c r="F7" s="137"/>
+      <c r="G7" s="137"/>
+      <c r="H7" s="137"/>
+      <c r="I7" s="137"/>
+      <c r="J7" s="137"/>
+      <c r="K7" s="137"/>
+      <c r="L7" s="137"/>
       <c r="M7" s="71"/>
       <c r="N7" s="70" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O7" s="72"/>
       <c r="P7" s="72"/>
@@ -2707,84 +2727,84 @@
       <c r="V7" s="73"/>
     </row>
     <row r="8" spans="1:22" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="133" t="s">
+      <c r="A8" s="124" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="137" t="s">
+      <c r="B8" s="128" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="124" t="s">
+      <c r="C8" s="115" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="116"/>
+      <c r="E8" s="117"/>
+      <c r="F8" s="112" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="125"/>
-      <c r="E8" s="126"/>
-      <c r="F8" s="121" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="122"/>
-      <c r="H8" s="123"/>
-      <c r="I8" s="119" t="s">
+      <c r="G8" s="113"/>
+      <c r="H8" s="114"/>
+      <c r="I8" s="111" t="s">
+        <v>41</v>
+      </c>
+      <c r="J8" s="99"/>
+      <c r="K8" s="120" t="s">
+        <v>38</v>
+      </c>
+      <c r="L8" s="145" t="s">
+        <v>38</v>
+      </c>
+      <c r="M8" s="122" t="s">
         <v>42</v>
       </c>
-      <c r="J8" s="120"/>
-      <c r="K8" s="129" t="s">
-        <v>39</v>
-      </c>
-      <c r="L8" s="112" t="s">
-        <v>39</v>
-      </c>
-      <c r="M8" s="131" t="s">
-        <v>43</v>
-      </c>
-      <c r="N8" s="135"/>
-      <c r="O8" s="99"/>
-      <c r="P8" s="99"/>
-      <c r="Q8" s="99"/>
-      <c r="R8" s="99"/>
-      <c r="S8" s="99"/>
-      <c r="T8" s="99"/>
-      <c r="U8" s="99"/>
-      <c r="V8" s="103"/>
+      <c r="N8" s="126"/>
+      <c r="O8" s="134"/>
+      <c r="P8" s="134"/>
+      <c r="Q8" s="134"/>
+      <c r="R8" s="134"/>
+      <c r="S8" s="134"/>
+      <c r="T8" s="134"/>
+      <c r="U8" s="134"/>
+      <c r="V8" s="147"/>
     </row>
     <row r="9" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="134"/>
-      <c r="B9" s="138"/>
+      <c r="A9" s="125"/>
+      <c r="B9" s="129"/>
       <c r="C9" s="74" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" s="74" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="74" t="s">
+      <c r="E9" s="74" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="74" t="s">
+      <c r="F9" s="75" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="75" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="75" t="s">
+        <v>20</v>
+      </c>
+      <c r="I9" s="76" t="s">
+        <v>30</v>
+      </c>
+      <c r="J9" s="76" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="75" t="s">
-        <v>19</v>
-      </c>
-      <c r="G9" s="75" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="75" t="s">
-        <v>21</v>
-      </c>
-      <c r="I9" s="76" t="s">
-        <v>31</v>
-      </c>
-      <c r="J9" s="76" t="s">
-        <v>22</v>
-      </c>
-      <c r="K9" s="130"/>
-      <c r="L9" s="113"/>
-      <c r="M9" s="132"/>
-      <c r="N9" s="136"/>
-      <c r="O9" s="100"/>
-      <c r="P9" s="100"/>
-      <c r="Q9" s="100"/>
-      <c r="R9" s="100"/>
-      <c r="S9" s="100"/>
-      <c r="T9" s="100"/>
-      <c r="U9" s="100"/>
-      <c r="V9" s="104"/>
+      <c r="K9" s="121"/>
+      <c r="L9" s="146"/>
+      <c r="M9" s="123"/>
+      <c r="N9" s="127"/>
+      <c r="O9" s="135"/>
+      <c r="P9" s="135"/>
+      <c r="Q9" s="135"/>
+      <c r="R9" s="135"/>
+      <c r="S9" s="135"/>
+      <c r="T9" s="135"/>
+      <c r="U9" s="135"/>
+      <c r="V9" s="148"/>
     </row>
     <row r="10" spans="1:22" s="42" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="49"/>
@@ -2825,11 +2845,11 @@
       <c r="M11" s="42"/>
     </row>
     <row r="12" spans="1:22" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="116" t="s">
-        <v>27</v>
-      </c>
-      <c r="B12" s="127"/>
-      <c r="C12" s="128"/>
+      <c r="A12" s="110" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="118"/>
+      <c r="C12" s="119"/>
       <c r="D12" s="62"/>
       <c r="E12" s="62"/>
       <c r="F12" s="62"/>
@@ -2841,7 +2861,7 @@
       <c r="L12" s="62"/>
       <c r="M12" s="60"/>
       <c r="N12" s="50" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O12" s="38"/>
       <c r="P12" s="38"/>
@@ -2853,50 +2873,50 @@
       <c r="V12" s="39"/>
     </row>
     <row r="13" spans="1:22" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="141" t="s">
+      <c r="A13" s="132" t="s">
+        <v>32</v>
+      </c>
+      <c r="B13" s="130" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="131"/>
+      <c r="M13" s="60"/>
+      <c r="N13" s="141" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="139" t="s">
-        <v>41</v>
-      </c>
-      <c r="C13" s="140"/>
-      <c r="M13" s="60"/>
-      <c r="N13" s="108" t="s">
+      <c r="O13" s="143" t="s">
         <v>34</v>
       </c>
-      <c r="O13" s="110" t="s">
-        <v>35</v>
-      </c>
-      <c r="P13" s="110" t="s">
-        <v>23</v>
-      </c>
-      <c r="Q13" s="114" t="s">
-        <v>17</v>
-      </c>
-      <c r="R13" s="96"/>
-      <c r="S13" s="96"/>
-      <c r="T13" s="98"/>
-      <c r="U13" s="99"/>
-      <c r="V13" s="101"/>
+      <c r="P13" s="143" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q13" s="108" t="s">
+        <v>16</v>
+      </c>
+      <c r="R13" s="149"/>
+      <c r="S13" s="149"/>
+      <c r="T13" s="151"/>
+      <c r="U13" s="134"/>
+      <c r="V13" s="152"/>
     </row>
     <row r="14" spans="1:22" ht="17.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="142"/>
+      <c r="A14" s="133"/>
       <c r="B14" s="77" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C14" s="78" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M14" s="60"/>
-      <c r="N14" s="109"/>
-      <c r="O14" s="111"/>
-      <c r="P14" s="111"/>
-      <c r="Q14" s="115"/>
-      <c r="R14" s="97"/>
-      <c r="S14" s="97"/>
-      <c r="T14" s="97"/>
-      <c r="U14" s="100"/>
-      <c r="V14" s="102"/>
+      <c r="N14" s="142"/>
+      <c r="O14" s="144"/>
+      <c r="P14" s="144"/>
+      <c r="Q14" s="109"/>
+      <c r="R14" s="150"/>
+      <c r="S14" s="150"/>
+      <c r="T14" s="150"/>
+      <c r="U14" s="135"/>
+      <c r="V14" s="153"/>
     </row>
     <row r="15" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="18"/>
@@ -2928,23 +2948,23 @@
       <c r="M16" s="48"/>
     </row>
     <row r="17" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="105" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="106"/>
-      <c r="C17" s="106"/>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
-      <c r="F17" s="106"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="106"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="107"/>
+      <c r="A17" s="138" t="s">
+        <v>28</v>
+      </c>
+      <c r="B17" s="139"/>
+      <c r="C17" s="139"/>
+      <c r="D17" s="139"/>
+      <c r="E17" s="139"/>
+      <c r="F17" s="139"/>
+      <c r="G17" s="139"/>
+      <c r="H17" s="139"/>
+      <c r="I17" s="139"/>
+      <c r="J17" s="139"/>
+      <c r="K17" s="139"/>
+      <c r="L17" s="140"/>
       <c r="M17" s="79"/>
       <c r="N17" s="51" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="O17" s="44"/>
       <c r="P17" s="44"/>
@@ -2956,84 +2976,84 @@
       <c r="V17" s="45"/>
     </row>
     <row r="18" spans="1:22" s="46" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="145" t="s">
+      <c r="A18" s="93" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" s="97" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="100" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="103"/>
+      <c r="E18" s="101"/>
+      <c r="F18" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="G18" s="103"/>
+      <c r="H18" s="101"/>
+      <c r="I18" s="100" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="101"/>
+      <c r="K18" s="97" t="s">
+        <v>0</v>
+      </c>
+      <c r="L18" s="106" t="s">
+        <v>0</v>
+      </c>
+      <c r="M18" s="104" t="s">
         <v>32</v>
       </c>
-      <c r="B18" s="149" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="151" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="154"/>
-      <c r="E18" s="152"/>
-      <c r="F18" s="153" t="s">
-        <v>38</v>
-      </c>
-      <c r="G18" s="154"/>
-      <c r="H18" s="152"/>
-      <c r="I18" s="151" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="152"/>
-      <c r="K18" s="149" t="s">
-        <v>0</v>
-      </c>
-      <c r="L18" s="157" t="s">
-        <v>0</v>
-      </c>
-      <c r="M18" s="155" t="s">
-        <v>33</v>
-      </c>
-      <c r="N18" s="147"/>
-      <c r="O18" s="92"/>
-      <c r="P18" s="92"/>
-      <c r="Q18" s="92"/>
-      <c r="R18" s="92"/>
-      <c r="S18" s="92"/>
-      <c r="T18" s="92"/>
-      <c r="U18" s="92"/>
-      <c r="V18" s="94"/>
+      <c r="N18" s="95"/>
+      <c r="O18" s="154"/>
+      <c r="P18" s="154"/>
+      <c r="Q18" s="154"/>
+      <c r="R18" s="154"/>
+      <c r="S18" s="154"/>
+      <c r="T18" s="154"/>
+      <c r="U18" s="154"/>
+      <c r="V18" s="156"/>
     </row>
     <row r="19" spans="1:22" s="46" customFormat="1" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="146"/>
-      <c r="B19" s="150"/>
+      <c r="A19" s="94"/>
+      <c r="B19" s="98"/>
       <c r="C19" s="80" t="s">
+        <v>18</v>
+      </c>
+      <c r="D19" s="80" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="80" t="s">
+      <c r="E19" s="80" t="s">
         <v>20</v>
       </c>
-      <c r="E19" s="80" t="s">
+      <c r="F19" s="81" t="s">
+        <v>18</v>
+      </c>
+      <c r="G19" s="81" t="s">
+        <v>19</v>
+      </c>
+      <c r="H19" s="81" t="s">
+        <v>20</v>
+      </c>
+      <c r="I19" s="80" t="s">
+        <v>30</v>
+      </c>
+      <c r="J19" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="F19" s="81" t="s">
-        <v>19</v>
-      </c>
-      <c r="G19" s="81" t="s">
-        <v>20</v>
-      </c>
-      <c r="H19" s="81" t="s">
-        <v>21</v>
-      </c>
-      <c r="I19" s="80" t="s">
-        <v>31</v>
-      </c>
-      <c r="J19" s="80" t="s">
-        <v>22</v>
-      </c>
-      <c r="K19" s="120"/>
-      <c r="L19" s="158"/>
-      <c r="M19" s="156"/>
-      <c r="N19" s="148"/>
-      <c r="O19" s="93"/>
-      <c r="P19" s="93"/>
-      <c r="Q19" s="93"/>
-      <c r="R19" s="93"/>
-      <c r="S19" s="93"/>
-      <c r="T19" s="93"/>
-      <c r="U19" s="93"/>
-      <c r="V19" s="95"/>
+      <c r="K19" s="99"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="105"/>
+      <c r="N19" s="96"/>
+      <c r="O19" s="155"/>
+      <c r="P19" s="155"/>
+      <c r="Q19" s="155"/>
+      <c r="R19" s="155"/>
+      <c r="S19" s="155"/>
+      <c r="T19" s="155"/>
+      <c r="U19" s="155"/>
+      <c r="V19" s="157"/>
     </row>
     <row r="20" spans="1:22" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="64"/>
@@ -5105,17 +5125,32 @@
     </row>
   </sheetData>
   <mergeCells count="49">
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="N18:N19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="K18:K19"/>
-    <mergeCell ref="I18:J18"/>
-    <mergeCell ref="F18:H18"/>
-    <mergeCell ref="M18:M19"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="L18:L19"/>
+    <mergeCell ref="T18:T19"/>
+    <mergeCell ref="U18:U19"/>
+    <mergeCell ref="V18:V19"/>
+    <mergeCell ref="O18:O19"/>
+    <mergeCell ref="P18:P19"/>
+    <mergeCell ref="Q18:Q19"/>
+    <mergeCell ref="R18:R19"/>
+    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="R13:R14"/>
+    <mergeCell ref="S13:S14"/>
+    <mergeCell ref="T13:T14"/>
+    <mergeCell ref="U13:U14"/>
+    <mergeCell ref="V13:V14"/>
+    <mergeCell ref="R8:R9"/>
+    <mergeCell ref="S8:S9"/>
+    <mergeCell ref="T8:T9"/>
+    <mergeCell ref="U8:U9"/>
+    <mergeCell ref="V8:V9"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="N13:N14"/>
+    <mergeCell ref="O13:O14"/>
+    <mergeCell ref="P13:P14"/>
+    <mergeCell ref="L8:L9"/>
+    <mergeCell ref="O8:O9"/>
+    <mergeCell ref="P8:P9"/>
     <mergeCell ref="Q13:Q14"/>
-    <mergeCell ref="A1:C1"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="F8:H8"/>
     <mergeCell ref="C8:E8"/>
@@ -5129,31 +5164,16 @@
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="Q8:Q9"/>
     <mergeCell ref="A7:L7"/>
-    <mergeCell ref="A17:L17"/>
-    <mergeCell ref="N13:N14"/>
-    <mergeCell ref="O13:O14"/>
-    <mergeCell ref="P13:P14"/>
-    <mergeCell ref="L8:L9"/>
-    <mergeCell ref="O8:O9"/>
-    <mergeCell ref="P8:P9"/>
-    <mergeCell ref="R8:R9"/>
-    <mergeCell ref="S8:S9"/>
-    <mergeCell ref="T8:T9"/>
-    <mergeCell ref="U8:U9"/>
-    <mergeCell ref="V8:V9"/>
-    <mergeCell ref="R13:R14"/>
-    <mergeCell ref="S13:S14"/>
-    <mergeCell ref="T13:T14"/>
-    <mergeCell ref="U13:U14"/>
-    <mergeCell ref="V13:V14"/>
-    <mergeCell ref="T18:T19"/>
-    <mergeCell ref="U18:U19"/>
-    <mergeCell ref="V18:V19"/>
-    <mergeCell ref="O18:O19"/>
-    <mergeCell ref="P18:P19"/>
-    <mergeCell ref="Q18:Q19"/>
-    <mergeCell ref="R18:R19"/>
-    <mergeCell ref="S18:S19"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="N18:N19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="K18:K19"/>
+    <mergeCell ref="I18:J18"/>
+    <mergeCell ref="F18:H18"/>
+    <mergeCell ref="M18:M19"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="L18:L19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -5182,44 +5202,44 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="21" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="161" t="s">
+      <c r="A1" s="160" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="163" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="164"/>
-      <c r="D1" s="164"/>
-      <c r="E1" s="163" t="s">
-        <v>42</v>
-      </c>
-      <c r="F1" s="164"/>
-      <c r="G1" s="159" t="s">
-        <v>39</v>
-      </c>
-      <c r="H1" s="112" t="s">
-        <v>39</v>
+      <c r="B1" s="162" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="163"/>
+      <c r="D1" s="163"/>
+      <c r="E1" s="162" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="163"/>
+      <c r="G1" s="158" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="145" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="54" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="162"/>
+      <c r="A2" s="161"/>
       <c r="B2" s="91" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="91" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="91" t="s">
+      <c r="D2" s="91" t="s">
         <v>20</v>
       </c>
-      <c r="D2" s="91" t="s">
+      <c r="E2" s="91" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="91" t="s">
         <v>21</v>
       </c>
-      <c r="E2" s="91" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="91" t="s">
-        <v>22</v>
-      </c>
-      <c r="G2" s="160"/>
-      <c r="H2" s="165"/>
+      <c r="G2" s="159"/>
+      <c r="H2" s="164"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="H3" s="53" t="e">
@@ -11265,16 +11285,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -11418,20 +11438,20 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="92" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" s="166" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -11439,17 +11459,17 @@
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
   </sheetData>

</xml_diff>